<commit_message>
Cleaned up the FinancialData class constructor
</commit_message>
<xml_diff>
--- a/Financial Modelling Prep Library/Company Financial Data/NVDA/annual/balance_sheets.xlsx
+++ b/Financial Modelling Prep Library/Company Financial Data/NVDA/annual/balance_sheets.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="155" uniqueCount="117">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="249" uniqueCount="168">
   <si>
     <t>date</t>
   </si>
@@ -181,6 +181,36 @@
     <t>index</t>
   </si>
   <si>
+    <t>NVDA-FY-2003</t>
+  </si>
+  <si>
+    <t>NVDA-FY-2004</t>
+  </si>
+  <si>
+    <t>NVDA-FY-2005</t>
+  </si>
+  <si>
+    <t>NVDA-FY-2006</t>
+  </si>
+  <si>
+    <t>NVDA-FY-2007</t>
+  </si>
+  <si>
+    <t>NVDA-FY-2008</t>
+  </si>
+  <si>
+    <t>NVDA-FY-2009</t>
+  </si>
+  <si>
+    <t>NVDA-FY-2010</t>
+  </si>
+  <si>
+    <t>NVDA-FY-2011</t>
+  </si>
+  <si>
+    <t>NVDA-FY-2012</t>
+  </si>
+  <si>
     <t>NVDA-FY-2013</t>
   </si>
   <si>
@@ -220,6 +250,36 @@
     <t>0001045810</t>
   </si>
   <si>
+    <t>2003-04-25</t>
+  </si>
+  <si>
+    <t>2004-01-31</t>
+  </si>
+  <si>
+    <t>2005-03-22</t>
+  </si>
+  <si>
+    <t>2006-03-16</t>
+  </si>
+  <si>
+    <t>2007-03-16</t>
+  </si>
+  <si>
+    <t>2008-01-31</t>
+  </si>
+  <si>
+    <t>2009-01-31</t>
+  </si>
+  <si>
+    <t>2010-03-18</t>
+  </si>
+  <si>
+    <t>2011-03-16</t>
+  </si>
+  <si>
+    <t>2012-03-13</t>
+  </si>
+  <si>
     <t>2013-03-12</t>
   </si>
   <si>
@@ -250,6 +310,36 @@
     <t>2022-03-18</t>
   </si>
   <si>
+    <t>2003-04-24 21:55:57</t>
+  </si>
+  <si>
+    <t>2004-01-30 19:00:00</t>
+  </si>
+  <si>
+    <t>2005-03-22 14:33:30</t>
+  </si>
+  <si>
+    <t>2006-03-16 17:08:37</t>
+  </si>
+  <si>
+    <t>2007-03-16 14:12:51</t>
+  </si>
+  <si>
+    <t>2008-01-30 19:00:00</t>
+  </si>
+  <si>
+    <t>2009-01-30 19:00:00</t>
+  </si>
+  <si>
+    <t>2010-03-17 19:16:55</t>
+  </si>
+  <si>
+    <t>2011-03-16 16:33:51</t>
+  </si>
+  <si>
+    <t>2012-03-13 16:56:38</t>
+  </si>
+  <si>
     <t>2013-03-12 17:03:06</t>
   </si>
   <si>
@@ -280,6 +370,36 @@
     <t>2022-02-15 19:00:00</t>
   </si>
   <si>
+    <t>2003</t>
+  </si>
+  <si>
+    <t>2004</t>
+  </si>
+  <si>
+    <t>2005</t>
+  </si>
+  <si>
+    <t>2006</t>
+  </si>
+  <si>
+    <t>2007</t>
+  </si>
+  <si>
+    <t>2008</t>
+  </si>
+  <si>
+    <t>2009</t>
+  </si>
+  <si>
+    <t>2010</t>
+  </si>
+  <si>
+    <t>2011</t>
+  </si>
+  <si>
+    <t>2012</t>
+  </si>
+  <si>
     <t>2013</t>
   </si>
   <si>
@@ -313,6 +433,27 @@
     <t>FY</t>
   </si>
   <si>
+    <t>https://www.sec.gov/Archives/edgar/data/1045810/000104596903001196/0001045969-03-001196-index.html</t>
+  </si>
+  <si>
+    <t>https://www.sec.gov/Archives/edgar/data/1045810/000104581005000008/0001045810-05-000008-index.html</t>
+  </si>
+  <si>
+    <t>https://www.sec.gov/Archives/edgar/data/1045810/000104581006000014/fy2006annualreportonform10-k.htm</t>
+  </si>
+  <si>
+    <t>https://www.sec.gov/Archives/edgar/data/1045810/000104581007000008/fy2007annualreportonform10-k.htm</t>
+  </si>
+  <si>
+    <t>https://www.sec.gov/Archives/edgar/data/1045810/000104581010000006/0001045810-10-000006-index.html</t>
+  </si>
+  <si>
+    <t>https://www.sec.gov/Archives/edgar/data/1045810/000104581011000015/fy2011form10k.htm</t>
+  </si>
+  <si>
+    <t>https://www.sec.gov/Archives/edgar/data/1045810/000104581012000013/0001045810-12-000013-index.html</t>
+  </si>
+  <si>
     <t>https://www.sec.gov/Archives/edgar/data/1045810/000104581013000008/0001045810-13-000008-index.html</t>
   </si>
   <si>
@@ -341,6 +482,18 @@
   </si>
   <si>
     <t>https://www.sec.gov/Archives/edgar/data/1045810/000104581022000036/0001045810-22-000036-index.htm</t>
+  </si>
+  <si>
+    <t>https://www.sec.gov/Archives/edgar/data/1045810/000104596903001196/d10k.htm</t>
+  </si>
+  <si>
+    <t>https://www.sec.gov/Archives/edgar/data/1045810/000104581005000008/annualreport.htm</t>
+  </si>
+  <si>
+    <t>https://www.sec.gov/Archives/edgar/data/1045810/000104581010000006/fy2010form10k.htm</t>
+  </si>
+  <si>
+    <t>https://www.sec.gov/Archives/edgar/data/1045810/000104581012000013/nvda-2012x10k.htm</t>
   </si>
   <si>
     <t>https://www.sec.gov/Archives/edgar/data/1045810/000104581013000008/nvda-2013x10k.htm</t>
@@ -739,7 +892,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:BC11"/>
+  <dimension ref="A1:BC21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -917,166 +1070,166 @@
         <v>55</v>
       </c>
       <c r="B2" s="2">
-        <v>41301</v>
+        <v>37647</v>
       </c>
       <c r="C2" t="s">
-        <v>65</v>
+        <v>75</v>
       </c>
       <c r="D2" t="s">
-        <v>66</v>
+        <v>76</v>
       </c>
       <c r="E2" t="s">
-        <v>67</v>
+        <v>77</v>
       </c>
       <c r="F2" t="s">
-        <v>68</v>
+        <v>78</v>
       </c>
       <c r="G2" t="s">
-        <v>78</v>
+        <v>98</v>
       </c>
       <c r="H2" t="s">
-        <v>88</v>
+        <v>118</v>
       </c>
       <c r="I2" t="s">
-        <v>98</v>
+        <v>138</v>
       </c>
       <c r="J2">
-        <v>732786000</v>
+        <v>346994000</v>
       </c>
       <c r="K2">
-        <v>2995097000</v>
+        <v>681419000</v>
       </c>
       <c r="L2">
-        <v>3727883000</v>
+        <v>1028413000</v>
       </c>
       <c r="M2">
-        <v>454252000</v>
+        <v>154501000</v>
       </c>
       <c r="N2">
-        <v>419686000</v>
+        <v>145046000</v>
       </c>
       <c r="O2">
-        <v>173437000</v>
+        <v>23642000</v>
       </c>
       <c r="P2">
-        <v>4775258000</v>
+        <v>1351602000</v>
       </c>
       <c r="Q2">
-        <v>576144000</v>
+        <v>135152000</v>
       </c>
       <c r="R2">
-        <v>641030000</v>
+        <v>0</v>
       </c>
       <c r="S2">
-        <v>312332000</v>
+        <v>76471000</v>
       </c>
       <c r="T2">
-        <v>953362000</v>
+        <v>76471000</v>
       </c>
       <c r="U2">
-        <v>10030000</v>
+        <v>0</v>
       </c>
       <c r="V2">
-        <v>3527000</v>
+        <v>43317000</v>
       </c>
       <c r="W2">
-        <v>93924000</v>
+        <v>10473000</v>
       </c>
       <c r="X2">
-        <v>1636987000</v>
+        <v>265413000</v>
       </c>
       <c r="Y2">
         <v>0</v>
       </c>
       <c r="Z2">
-        <v>6412245000</v>
+        <v>1617015000</v>
       </c>
       <c r="AA2">
-        <v>356428000</v>
+        <v>141129000</v>
       </c>
       <c r="AB2">
-        <v>0</v>
+        <v>5676000</v>
       </c>
       <c r="AC2">
-        <v>3173000</v>
+        <v>0</v>
       </c>
       <c r="AD2">
-        <v>273605000</v>
+        <v>0</v>
       </c>
       <c r="AE2">
-        <v>343017000</v>
+        <v>232643000</v>
       </c>
       <c r="AF2">
-        <v>976223000</v>
+        <v>379448000</v>
       </c>
       <c r="AG2">
-        <v>18998000</v>
+        <v>304880000</v>
       </c>
       <c r="AH2">
-        <v>236152000</v>
+        <v>0</v>
       </c>
       <c r="AI2">
-        <v>192950000</v>
+        <v>0</v>
       </c>
       <c r="AJ2">
-        <v>160219000</v>
+        <v>0</v>
       </c>
       <c r="AK2">
-        <v>608319000</v>
+        <v>304880000</v>
       </c>
       <c r="AL2">
         <v>0</v>
       </c>
       <c r="AM2">
-        <v>18998000</v>
+        <v>4880000</v>
       </c>
       <c r="AN2">
-        <v>1584542000</v>
+        <v>684328000</v>
       </c>
       <c r="AO2">
         <v>0</v>
       </c>
       <c r="AP2">
-        <v>720000</v>
+        <v>158000</v>
       </c>
       <c r="AQ2">
-        <v>3246088000</v>
+        <v>397739000</v>
       </c>
       <c r="AR2">
-        <v>9981000</v>
+        <v>3760000</v>
       </c>
       <c r="AS2">
-        <v>1570914000</v>
+        <v>531030000</v>
       </c>
       <c r="AT2">
-        <v>4827703000</v>
+        <v>932687000</v>
       </c>
       <c r="AU2">
-        <v>4827703000</v>
+        <v>932687000</v>
       </c>
       <c r="AV2">
-        <v>6412245000</v>
+        <v>1617015000</v>
       </c>
       <c r="AW2">
         <v>0</v>
       </c>
       <c r="AX2">
-        <v>6412245000</v>
+        <v>1617015000</v>
       </c>
       <c r="AY2">
-        <v>3005127000</v>
+        <v>0</v>
       </c>
       <c r="AZ2">
-        <v>18998000</v>
+        <v>310556000</v>
       </c>
       <c r="BA2">
-        <v>-713788000</v>
+        <v>-36438000</v>
       </c>
       <c r="BB2" s="3" t="s">
-        <v>99</v>
+        <v>139</v>
       </c>
       <c r="BC2" s="3" t="s">
-        <v>109</v>
+        <v>156</v>
       </c>
     </row>
     <row r="3" spans="1:55">
@@ -1084,61 +1237,61 @@
         <v>56</v>
       </c>
       <c r="B3" s="2">
-        <v>41665</v>
+        <v>38017</v>
       </c>
       <c r="C3" t="s">
-        <v>65</v>
+        <v>75</v>
       </c>
       <c r="D3" t="s">
-        <v>66</v>
+        <v>76</v>
       </c>
       <c r="E3" t="s">
-        <v>67</v>
+        <v>77</v>
       </c>
       <c r="F3" t="s">
-        <v>69</v>
+        <v>79</v>
       </c>
       <c r="G3" t="s">
-        <v>79</v>
+        <v>99</v>
       </c>
       <c r="H3" t="s">
-        <v>89</v>
+        <v>119</v>
       </c>
       <c r="I3" t="s">
-        <v>98</v>
+        <v>138</v>
       </c>
       <c r="J3">
-        <v>1151587000</v>
+        <v>214422000</v>
       </c>
       <c r="K3">
-        <v>3520223000</v>
+        <v>389621000</v>
       </c>
       <c r="L3">
-        <v>4671810000</v>
+        <v>604043000</v>
       </c>
       <c r="M3">
-        <v>426357000</v>
+        <v>196631000</v>
       </c>
       <c r="N3">
-        <v>387765000</v>
+        <v>234238000</v>
       </c>
       <c r="O3">
-        <v>138779000</v>
+        <v>17800000</v>
       </c>
       <c r="P3">
-        <v>5624711000</v>
+        <v>1052712000</v>
       </c>
       <c r="Q3">
-        <v>582740000</v>
+        <v>190029000</v>
       </c>
       <c r="R3">
-        <v>643179000</v>
+        <v>0</v>
       </c>
       <c r="S3">
-        <v>296012000</v>
+        <v>148872000</v>
       </c>
       <c r="T3">
-        <v>939191000</v>
+        <v>148872000</v>
       </c>
       <c r="U3">
         <v>0</v>
@@ -1147,103 +1300,97 @@
         <v>0</v>
       </c>
       <c r="W3">
-        <v>104252000</v>
+        <v>7731000</v>
       </c>
       <c r="X3">
-        <v>1626183000</v>
+        <v>346632000</v>
       </c>
       <c r="Y3">
         <v>0</v>
       </c>
       <c r="Z3">
-        <v>7250894000</v>
+        <v>1399344000</v>
       </c>
       <c r="AA3">
-        <v>324391000</v>
+        <v>185342000</v>
       </c>
       <c r="AB3">
-        <v>0</v>
+        <v>4015000</v>
       </c>
       <c r="AC3">
-        <v>2378000</v>
+        <v>0</v>
       </c>
       <c r="AD3">
-        <v>282405000</v>
+        <v>0</v>
       </c>
       <c r="AE3">
-        <v>336322000</v>
+        <v>144755000</v>
       </c>
       <c r="AF3">
-        <v>945496000</v>
+        <v>334112000</v>
       </c>
       <c r="AG3">
-        <v>1373875000</v>
+        <v>856000</v>
       </c>
       <c r="AH3">
-        <v>172199000</v>
+        <v>0</v>
       </c>
       <c r="AI3">
-        <v>157953000</v>
+        <v>8609000</v>
       </c>
       <c r="AJ3">
-        <v>144973000</v>
+        <v>4582000</v>
       </c>
       <c r="AK3">
-        <v>1849000000</v>
+        <v>14047000</v>
       </c>
       <c r="AL3">
         <v>0</v>
       </c>
       <c r="AM3">
-        <v>17500000</v>
+        <v>856000</v>
       </c>
       <c r="AN3">
-        <v>2794496000</v>
+        <v>348159000</v>
       </c>
       <c r="AO3">
         <v>0</v>
       </c>
       <c r="AP3">
-        <v>732000</v>
+        <v>164000</v>
       </c>
       <c r="AQ3">
-        <v>3504742000</v>
+        <v>472158000</v>
       </c>
       <c r="AR3">
-        <v>4877000</v>
+        <v>-4618000</v>
       </c>
       <c r="AS3">
-        <v>946047000</v>
+        <v>583481000</v>
       </c>
       <c r="AT3">
-        <v>4456398000</v>
+        <v>1051185000</v>
       </c>
       <c r="AU3">
-        <v>4456398000</v>
+        <v>1051185000</v>
       </c>
       <c r="AV3">
-        <v>7250894000</v>
+        <v>1399344000</v>
       </c>
       <c r="AW3">
         <v>0</v>
       </c>
       <c r="AX3">
-        <v>7250894000</v>
+        <v>1399344000</v>
       </c>
       <c r="AY3">
         <v>0</v>
       </c>
       <c r="AZ3">
-        <v>1373875000</v>
+        <v>4871000</v>
       </c>
       <c r="BA3">
-        <v>222288000</v>
-      </c>
-      <c r="BB3" s="3" t="s">
-        <v>100</v>
-      </c>
-      <c r="BC3" s="3" t="s">
-        <v>100</v>
+        <v>-209551000</v>
       </c>
     </row>
     <row r="4" spans="1:55">
@@ -1251,61 +1398,61 @@
         <v>57</v>
       </c>
       <c r="B4" s="2">
-        <v>42029</v>
+        <v>38382</v>
       </c>
       <c r="C4" t="s">
-        <v>65</v>
+        <v>75</v>
       </c>
       <c r="D4" t="s">
-        <v>66</v>
+        <v>76</v>
       </c>
       <c r="E4" t="s">
-        <v>67</v>
+        <v>77</v>
       </c>
       <c r="F4" t="s">
-        <v>70</v>
+        <v>80</v>
       </c>
       <c r="G4" t="s">
-        <v>80</v>
+        <v>100</v>
       </c>
       <c r="H4" t="s">
-        <v>90</v>
+        <v>120</v>
       </c>
       <c r="I4" t="s">
-        <v>98</v>
+        <v>138</v>
       </c>
       <c r="J4">
-        <v>496654000</v>
+        <v>208512000</v>
       </c>
       <c r="K4">
-        <v>4126685000</v>
+        <v>461533000</v>
       </c>
       <c r="L4">
-        <v>4623339000</v>
+        <v>670045000</v>
       </c>
       <c r="M4">
-        <v>473637000</v>
+        <v>296279000</v>
       </c>
       <c r="N4">
-        <v>482893000</v>
+        <v>315518000</v>
       </c>
       <c r="O4">
-        <v>133428000</v>
+        <v>23084000</v>
       </c>
       <c r="P4">
-        <v>5713297000</v>
+        <v>1304926000</v>
       </c>
       <c r="Q4">
-        <v>557282000</v>
+        <v>178955000</v>
       </c>
       <c r="R4">
-        <v>618179000</v>
+        <v>0</v>
       </c>
       <c r="S4">
-        <v>221714000</v>
+        <v>135621000</v>
       </c>
       <c r="T4">
-        <v>839893000</v>
+        <v>135621000</v>
       </c>
       <c r="U4">
         <v>0</v>
@@ -1314,103 +1461,103 @@
         <v>0</v>
       </c>
       <c r="W4">
-        <v>90896000</v>
+        <v>9034000</v>
       </c>
       <c r="X4">
-        <v>1488071000</v>
+        <v>323610000</v>
       </c>
       <c r="Y4">
         <v>0</v>
       </c>
       <c r="Z4">
-        <v>7201368000</v>
+        <v>1628536000</v>
       </c>
       <c r="AA4">
-        <v>293223000</v>
+        <v>238223000</v>
       </c>
       <c r="AB4">
-        <v>0</v>
+        <v>856000</v>
       </c>
       <c r="AC4">
-        <v>2810000</v>
+        <v>0</v>
       </c>
       <c r="AD4">
-        <v>292735000</v>
+        <v>11500000</v>
       </c>
       <c r="AE4">
-        <v>307262000</v>
+        <v>170577000</v>
       </c>
       <c r="AF4">
-        <v>896030000</v>
+        <v>421156000</v>
       </c>
       <c r="AG4">
-        <v>1398428000</v>
+        <v>0</v>
       </c>
       <c r="AH4">
-        <v>107838000</v>
+        <v>0</v>
       </c>
       <c r="AI4">
-        <v>232307000</v>
+        <v>20754000</v>
       </c>
       <c r="AJ4">
-        <v>148783000</v>
+        <v>8358000</v>
       </c>
       <c r="AK4">
-        <v>1887356000</v>
+        <v>29112000</v>
       </c>
       <c r="AL4">
         <v>0</v>
       </c>
       <c r="AM4">
-        <v>14086000</v>
+        <v>0</v>
       </c>
       <c r="AN4">
-        <v>2783386000</v>
+        <v>450268000</v>
       </c>
       <c r="AO4">
         <v>0</v>
       </c>
       <c r="AP4">
-        <v>754000</v>
+        <v>169000</v>
       </c>
       <c r="AQ4">
-        <v>3948877000</v>
+        <v>572514000</v>
       </c>
       <c r="AR4">
-        <v>7844000</v>
+        <v>-6389000</v>
       </c>
       <c r="AS4">
-        <v>460507000</v>
+        <v>611974000</v>
       </c>
       <c r="AT4">
-        <v>4417982000</v>
+        <v>1178268000</v>
       </c>
       <c r="AU4">
-        <v>4417982000</v>
+        <v>1178268000</v>
       </c>
       <c r="AV4">
-        <v>7201368000</v>
+        <v>1628536000</v>
       </c>
       <c r="AW4">
         <v>0</v>
       </c>
       <c r="AX4">
-        <v>7201368000</v>
+        <v>1628536000</v>
       </c>
       <c r="AY4">
         <v>0</v>
       </c>
       <c r="AZ4">
-        <v>1398428000</v>
+        <v>856000</v>
       </c>
       <c r="BA4">
-        <v>901774000</v>
+        <v>-207656000</v>
       </c>
       <c r="BB4" s="3" t="s">
-        <v>101</v>
+        <v>140</v>
       </c>
       <c r="BC4" s="3" t="s">
-        <v>101</v>
+        <v>157</v>
       </c>
     </row>
     <row r="5" spans="1:55">
@@ -1418,61 +1565,61 @@
         <v>58</v>
       </c>
       <c r="B5" s="2">
-        <v>42400</v>
+        <v>38746</v>
       </c>
       <c r="C5" t="s">
-        <v>65</v>
+        <v>75</v>
       </c>
       <c r="D5" t="s">
-        <v>66</v>
+        <v>76</v>
       </c>
       <c r="E5" t="s">
-        <v>67</v>
+        <v>77</v>
       </c>
       <c r="F5" t="s">
-        <v>71</v>
+        <v>81</v>
       </c>
       <c r="G5" t="s">
-        <v>81</v>
+        <v>101</v>
       </c>
       <c r="H5" t="s">
-        <v>91</v>
+        <v>121</v>
       </c>
       <c r="I5" t="s">
-        <v>98</v>
+        <v>138</v>
       </c>
       <c r="J5">
-        <v>596000000</v>
+        <v>551756000</v>
       </c>
       <c r="K5">
-        <v>4441000000</v>
+        <v>398418000</v>
       </c>
       <c r="L5">
-        <v>5037000000</v>
+        <v>950174000</v>
       </c>
       <c r="M5">
-        <v>505000000</v>
+        <v>318186000</v>
       </c>
       <c r="N5">
-        <v>418000000</v>
+        <v>254792000</v>
       </c>
       <c r="O5">
-        <v>93000000</v>
+        <v>25780000</v>
       </c>
       <c r="P5">
-        <v>6053000000</v>
+        <v>1548932000</v>
       </c>
       <c r="Q5">
-        <v>466000000</v>
+        <v>178152000</v>
       </c>
       <c r="R5">
-        <v>618000000</v>
+        <v>0</v>
       </c>
       <c r="S5">
-        <v>166000000</v>
+        <v>160738000</v>
       </c>
       <c r="T5">
-        <v>784000000</v>
+        <v>160738000</v>
       </c>
       <c r="U5">
         <v>0</v>
@@ -1481,103 +1628,103 @@
         <v>0</v>
       </c>
       <c r="W5">
-        <v>67000000</v>
+        <v>27477000</v>
       </c>
       <c r="X5">
-        <v>1317000000</v>
+        <v>366367000</v>
       </c>
       <c r="Y5">
         <v>0</v>
       </c>
       <c r="Z5">
-        <v>7370000000</v>
+        <v>1915299000</v>
       </c>
       <c r="AA5">
-        <v>296000000</v>
+        <v>179395000</v>
       </c>
       <c r="AB5">
-        <v>1500000000</v>
+        <v>0</v>
       </c>
       <c r="AC5">
-        <v>2000000</v>
+        <v>0</v>
       </c>
       <c r="AD5">
-        <v>322000000</v>
+        <v>0</v>
       </c>
       <c r="AE5">
-        <v>318000000</v>
+        <v>259264000</v>
       </c>
       <c r="AF5">
-        <v>2438000000</v>
+        <v>438659000</v>
       </c>
       <c r="AG5">
-        <v>10000000</v>
+        <v>0</v>
       </c>
       <c r="AH5">
-        <v>44000000</v>
+        <v>0</v>
       </c>
       <c r="AI5">
-        <v>301000000</v>
+        <v>8260000</v>
       </c>
       <c r="AJ5">
-        <v>108000000</v>
+        <v>10624000</v>
       </c>
       <c r="AK5">
-        <v>463000000</v>
+        <v>18884000</v>
       </c>
       <c r="AL5">
         <v>0</v>
       </c>
       <c r="AM5">
-        <v>10000000</v>
+        <v>0</v>
       </c>
       <c r="AN5">
-        <v>2901000000</v>
+        <v>457543000</v>
       </c>
       <c r="AO5">
         <v>0</v>
       </c>
       <c r="AP5">
-        <v>1000000</v>
+        <v>180000</v>
       </c>
       <c r="AQ5">
-        <v>4350000000</v>
+        <v>875100000</v>
       </c>
       <c r="AR5">
-        <v>-4000000</v>
+        <v>-3633000</v>
       </c>
       <c r="AS5">
-        <v>122000000</v>
+        <v>586109000</v>
       </c>
       <c r="AT5">
-        <v>4469000000</v>
+        <v>1457756000</v>
       </c>
       <c r="AU5">
-        <v>4469000000</v>
+        <v>1457756000</v>
       </c>
       <c r="AV5">
-        <v>7370000000</v>
+        <v>1915299000</v>
       </c>
       <c r="AW5">
         <v>0</v>
       </c>
       <c r="AX5">
-        <v>7370000000</v>
+        <v>1915299000</v>
       </c>
       <c r="AY5">
         <v>0</v>
       </c>
       <c r="AZ5">
-        <v>1510000000</v>
+        <v>0</v>
       </c>
       <c r="BA5">
-        <v>914000000</v>
+        <v>-551756000</v>
       </c>
       <c r="BB5" s="3" t="s">
-        <v>102</v>
+        <v>141</v>
       </c>
       <c r="BC5" s="3" t="s">
-        <v>110</v>
+        <v>141</v>
       </c>
     </row>
     <row r="6" spans="1:55">
@@ -1585,166 +1732,166 @@
         <v>59</v>
       </c>
       <c r="B6" s="2">
-        <v>42764</v>
+        <v>39110</v>
       </c>
       <c r="C6" t="s">
-        <v>65</v>
+        <v>75</v>
       </c>
       <c r="D6" t="s">
-        <v>66</v>
+        <v>76</v>
       </c>
       <c r="E6" t="s">
-        <v>67</v>
+        <v>77</v>
       </c>
       <c r="F6" t="s">
-        <v>72</v>
+        <v>82</v>
       </c>
       <c r="G6" t="s">
-        <v>82</v>
+        <v>102</v>
       </c>
       <c r="H6" t="s">
-        <v>92</v>
+        <v>122</v>
       </c>
       <c r="I6" t="s">
-        <v>98</v>
+        <v>138</v>
       </c>
       <c r="J6">
-        <v>1766000000</v>
+        <v>544414000</v>
       </c>
       <c r="K6">
-        <v>5032000000</v>
+        <v>573436000</v>
       </c>
       <c r="L6">
-        <v>6798000000</v>
+        <v>1117850000</v>
       </c>
       <c r="M6">
-        <v>826000000</v>
+        <v>518680000</v>
       </c>
       <c r="N6">
-        <v>794000000</v>
+        <v>354680000</v>
       </c>
       <c r="O6">
-        <v>118000000</v>
+        <v>40560000</v>
       </c>
       <c r="P6">
-        <v>8536000000</v>
+        <v>2031770000</v>
       </c>
       <c r="Q6">
-        <v>521000000</v>
+        <v>260828000</v>
       </c>
       <c r="R6">
-        <v>618000000</v>
+        <v>301425000</v>
       </c>
       <c r="S6">
-        <v>104000000</v>
+        <v>45511000</v>
       </c>
       <c r="T6">
-        <v>722000000</v>
+        <v>346936000</v>
       </c>
       <c r="U6">
         <v>0</v>
       </c>
       <c r="V6">
-        <v>0</v>
+        <v>7380000</v>
       </c>
       <c r="W6">
-        <v>62000000</v>
+        <v>28349000</v>
       </c>
       <c r="X6">
-        <v>1305000000</v>
+        <v>643493000</v>
       </c>
       <c r="Y6">
         <v>0</v>
       </c>
       <c r="Z6">
-        <v>9841000000</v>
+        <v>2675263000</v>
       </c>
       <c r="AA6">
-        <v>485000000</v>
+        <v>272075000</v>
       </c>
       <c r="AB6">
-        <v>827000000</v>
+        <v>0</v>
       </c>
       <c r="AC6">
-        <v>4000000</v>
+        <v>0</v>
       </c>
       <c r="AD6">
-        <v>85000000</v>
+        <v>1180000</v>
       </c>
       <c r="AE6">
-        <v>418000000</v>
+        <v>365552000</v>
       </c>
       <c r="AF6">
-        <v>1819000000</v>
+        <v>638807000</v>
       </c>
       <c r="AG6">
-        <v>1989000000</v>
+        <v>0</v>
       </c>
       <c r="AH6">
-        <v>4000000</v>
+        <v>0</v>
       </c>
       <c r="AI6">
-        <v>141000000</v>
+        <v>0</v>
       </c>
       <c r="AJ6">
-        <v>126000000</v>
+        <v>29537000</v>
       </c>
       <c r="AK6">
-        <v>2260000000</v>
+        <v>29537000</v>
       </c>
       <c r="AL6">
         <v>0</v>
       </c>
       <c r="AM6">
-        <v>6000000</v>
+        <v>0</v>
       </c>
       <c r="AN6">
-        <v>4079000000</v>
+        <v>668344000</v>
       </c>
       <c r="AO6">
         <v>0</v>
       </c>
       <c r="AP6">
-        <v>1000000</v>
+        <v>388000</v>
       </c>
       <c r="AQ6">
-        <v>6108000000</v>
+        <v>1196565000</v>
       </c>
       <c r="AR6">
-        <v>-16000000</v>
+        <v>1436000</v>
       </c>
       <c r="AS6">
-        <v>-331000000</v>
+        <v>808530000</v>
       </c>
       <c r="AT6">
-        <v>5762000000</v>
+        <v>2006919000</v>
       </c>
       <c r="AU6">
-        <v>5762000000</v>
+        <v>2006919000</v>
       </c>
       <c r="AV6">
-        <v>9841000000</v>
+        <v>2675263000</v>
       </c>
       <c r="AW6">
         <v>0</v>
       </c>
       <c r="AX6">
-        <v>9841000000</v>
+        <v>2675263000</v>
       </c>
       <c r="AY6">
         <v>0</v>
       </c>
       <c r="AZ6">
-        <v>2816000000</v>
+        <v>0</v>
       </c>
       <c r="BA6">
-        <v>1050000000</v>
+        <v>-544414000</v>
       </c>
       <c r="BB6" s="3" t="s">
-        <v>103</v>
+        <v>142</v>
       </c>
       <c r="BC6" s="3" t="s">
-        <v>111</v>
+        <v>142</v>
       </c>
     </row>
     <row r="7" spans="1:55">
@@ -1752,61 +1899,61 @@
         <v>60</v>
       </c>
       <c r="B7" s="2">
-        <v>43128</v>
+        <v>39478</v>
       </c>
       <c r="C7" t="s">
-        <v>65</v>
+        <v>75</v>
       </c>
       <c r="D7" t="s">
-        <v>66</v>
+        <v>76</v>
       </c>
       <c r="E7" t="s">
-        <v>67</v>
+        <v>77</v>
       </c>
       <c r="F7" t="s">
-        <v>73</v>
+        <v>83</v>
       </c>
       <c r="G7" t="s">
-        <v>83</v>
+        <v>103</v>
       </c>
       <c r="H7" t="s">
-        <v>93</v>
+        <v>123</v>
       </c>
       <c r="I7" t="s">
-        <v>98</v>
+        <v>138</v>
       </c>
       <c r="J7">
-        <v>4002000000</v>
+        <v>726969000</v>
       </c>
       <c r="K7">
-        <v>3106000000</v>
+        <v>1082509000</v>
       </c>
       <c r="L7">
-        <v>7108000000</v>
+        <v>1809478000</v>
       </c>
       <c r="M7">
-        <v>1265000000</v>
+        <v>666494000</v>
       </c>
       <c r="N7">
-        <v>796000000</v>
+        <v>358521000</v>
       </c>
       <c r="O7">
-        <v>86000000</v>
+        <v>54336000</v>
       </c>
       <c r="P7">
-        <v>9255000000</v>
+        <v>2888829000</v>
       </c>
       <c r="Q7">
-        <v>997000000</v>
+        <v>359808000</v>
       </c>
       <c r="R7">
-        <v>618000000</v>
+        <v>354057000</v>
       </c>
       <c r="S7">
-        <v>52000000</v>
+        <v>106926000</v>
       </c>
       <c r="T7">
-        <v>670000000</v>
+        <v>460983000</v>
       </c>
       <c r="U7">
         <v>0</v>
@@ -1815,49 +1962,49 @@
         <v>0</v>
       </c>
       <c r="W7">
-        <v>319000000</v>
+        <v>38051000</v>
       </c>
       <c r="X7">
-        <v>1986000000</v>
+        <v>858842000</v>
       </c>
       <c r="Y7">
         <v>0</v>
       </c>
       <c r="Z7">
-        <v>11241000000</v>
+        <v>3747671000</v>
       </c>
       <c r="AA7">
-        <v>596000000</v>
+        <v>492099000</v>
       </c>
       <c r="AB7">
-        <v>15000000</v>
+        <v>0</v>
       </c>
       <c r="AC7">
-        <v>33000000</v>
+        <v>0</v>
       </c>
       <c r="AD7">
-        <v>53000000</v>
+        <v>5856000</v>
       </c>
       <c r="AE7">
-        <v>456000000</v>
+        <v>469206000</v>
       </c>
       <c r="AF7">
-        <v>1153000000</v>
+        <v>967161000</v>
       </c>
       <c r="AG7">
-        <v>1985000000</v>
+        <v>0</v>
       </c>
       <c r="AH7">
-        <v>15000000</v>
+        <v>0</v>
       </c>
       <c r="AI7">
-        <v>18000000</v>
+        <v>86900000</v>
       </c>
       <c r="AJ7">
-        <v>599000000</v>
+        <v>75698000</v>
       </c>
       <c r="AK7">
-        <v>2617000000</v>
+        <v>162598000</v>
       </c>
       <c r="AL7">
         <v>0</v>
@@ -1866,52 +2013,46 @@
         <v>0</v>
       </c>
       <c r="AN7">
-        <v>3770000000</v>
+        <v>1129759000</v>
       </c>
       <c r="AO7">
         <v>0</v>
       </c>
       <c r="AP7">
-        <v>1000000</v>
+        <v>619000</v>
       </c>
       <c r="AQ7">
-        <v>8787000000</v>
+        <v>1994210000</v>
       </c>
       <c r="AR7">
-        <v>-18000000</v>
+        <v>8034000</v>
       </c>
       <c r="AS7">
-        <v>-1299000000</v>
+        <v>615049000</v>
       </c>
       <c r="AT7">
-        <v>7471000000</v>
+        <v>2617912000</v>
       </c>
       <c r="AU7">
-        <v>7471000000</v>
+        <v>2617912000</v>
       </c>
       <c r="AV7">
-        <v>11241000000</v>
+        <v>3747671000</v>
       </c>
       <c r="AW7">
         <v>0</v>
       </c>
       <c r="AX7">
-        <v>11241000000</v>
+        <v>3747671000</v>
       </c>
       <c r="AY7">
         <v>0</v>
       </c>
       <c r="AZ7">
-        <v>2000000000</v>
+        <v>0</v>
       </c>
       <c r="BA7">
-        <v>-2002000000</v>
-      </c>
-      <c r="BB7" s="3" t="s">
-        <v>104</v>
-      </c>
-      <c r="BC7" s="3" t="s">
-        <v>112</v>
+        <v>-726969000</v>
       </c>
     </row>
     <row r="8" spans="1:55">
@@ -1919,61 +2060,61 @@
         <v>61</v>
       </c>
       <c r="B8" s="2">
-        <v>43492</v>
+        <v>39844</v>
       </c>
       <c r="C8" t="s">
-        <v>65</v>
+        <v>75</v>
       </c>
       <c r="D8" t="s">
-        <v>66</v>
+        <v>76</v>
       </c>
       <c r="E8" t="s">
-        <v>67</v>
+        <v>77</v>
       </c>
       <c r="F8" t="s">
-        <v>74</v>
+        <v>84</v>
       </c>
       <c r="G8" t="s">
-        <v>84</v>
+        <v>104</v>
       </c>
       <c r="H8" t="s">
-        <v>94</v>
+        <v>124</v>
       </c>
       <c r="I8" t="s">
-        <v>98</v>
+        <v>138</v>
       </c>
       <c r="J8">
-        <v>782000000</v>
+        <v>417688000</v>
       </c>
       <c r="K8">
-        <v>6640000000</v>
+        <v>837702000</v>
       </c>
       <c r="L8">
-        <v>7422000000</v>
+        <v>1255390000</v>
       </c>
       <c r="M8">
-        <v>1424000000</v>
+        <v>318435000</v>
       </c>
       <c r="N8">
-        <v>1575000000</v>
+        <v>537834000</v>
       </c>
       <c r="O8">
-        <v>136000000</v>
+        <v>56299000</v>
       </c>
       <c r="P8">
-        <v>10557000000</v>
+        <v>2167958000</v>
       </c>
       <c r="Q8">
-        <v>1404000000</v>
+        <v>625798000</v>
       </c>
       <c r="R8">
-        <v>618000000</v>
+        <v>369844000</v>
       </c>
       <c r="S8">
-        <v>45000000</v>
+        <v>147101000</v>
       </c>
       <c r="T8">
-        <v>663000000</v>
+        <v>516945000</v>
       </c>
       <c r="U8">
         <v>0</v>
@@ -1982,103 +2123,97 @@
         <v>0</v>
       </c>
       <c r="W8">
-        <v>668000000</v>
+        <v>40026000</v>
       </c>
       <c r="X8">
-        <v>2735000000</v>
+        <v>1182769000</v>
       </c>
       <c r="Y8">
         <v>0</v>
       </c>
       <c r="Z8">
-        <v>13292000000</v>
+        <v>3350727000</v>
       </c>
       <c r="AA8">
-        <v>511000000</v>
+        <v>218864000</v>
       </c>
       <c r="AB8">
         <v>0</v>
       </c>
       <c r="AC8">
-        <v>91000000</v>
+        <v>0</v>
       </c>
       <c r="AD8">
-        <v>92000000</v>
+        <v>0</v>
       </c>
       <c r="AE8">
-        <v>635000000</v>
+        <v>559727000</v>
       </c>
       <c r="AF8">
-        <v>1329000000</v>
+        <v>778591000</v>
       </c>
       <c r="AG8">
-        <v>1988000000</v>
+        <v>25634000</v>
       </c>
       <c r="AH8">
-        <v>46000000</v>
+        <v>0</v>
       </c>
       <c r="AI8">
-        <v>19000000</v>
+        <v>0</v>
       </c>
       <c r="AJ8">
-        <v>568000000</v>
+        <v>151850000</v>
       </c>
       <c r="AK8">
-        <v>2621000000</v>
+        <v>177484000</v>
       </c>
       <c r="AL8">
         <v>0</v>
       </c>
       <c r="AM8">
-        <v>0</v>
+        <v>25634000</v>
       </c>
       <c r="AN8">
-        <v>3950000000</v>
+        <v>956075000</v>
       </c>
       <c r="AO8">
         <v>0</v>
       </c>
       <c r="AP8">
-        <v>1000000</v>
+        <v>629000</v>
       </c>
       <c r="AQ8">
-        <v>12565000000</v>
+        <v>1964169000</v>
       </c>
       <c r="AR8">
-        <v>-12000000</v>
+        <v>3865000</v>
       </c>
       <c r="AS8">
-        <v>-3212000000</v>
+        <v>425989000</v>
       </c>
       <c r="AT8">
-        <v>9342000000</v>
+        <v>2394652000</v>
       </c>
       <c r="AU8">
-        <v>9342000000</v>
+        <v>2394652000</v>
       </c>
       <c r="AV8">
-        <v>13292000000</v>
+        <v>3350727000</v>
       </c>
       <c r="AW8">
         <v>0</v>
       </c>
       <c r="AX8">
-        <v>13292000000</v>
+        <v>3350727000</v>
       </c>
       <c r="AY8">
         <v>0</v>
       </c>
       <c r="AZ8">
-        <v>1988000000</v>
+        <v>25634000</v>
       </c>
       <c r="BA8">
-        <v>1206000000</v>
-      </c>
-      <c r="BB8" s="3" t="s">
-        <v>105</v>
-      </c>
-      <c r="BC8" s="3" t="s">
-        <v>113</v>
+        <v>-392054000</v>
       </c>
     </row>
     <row r="9" spans="1:55">
@@ -2086,166 +2221,166 @@
         <v>62</v>
       </c>
       <c r="B9" s="2">
-        <v>43856</v>
+        <v>40209</v>
       </c>
       <c r="C9" t="s">
-        <v>65</v>
+        <v>75</v>
       </c>
       <c r="D9" t="s">
-        <v>66</v>
+        <v>76</v>
       </c>
       <c r="E9" t="s">
-        <v>67</v>
+        <v>77</v>
       </c>
       <c r="F9" t="s">
-        <v>75</v>
+        <v>85</v>
       </c>
       <c r="G9" t="s">
-        <v>85</v>
+        <v>105</v>
       </c>
       <c r="H9" t="s">
-        <v>95</v>
+        <v>125</v>
       </c>
       <c r="I9" t="s">
-        <v>98</v>
+        <v>138</v>
       </c>
       <c r="J9">
-        <v>10896000000</v>
+        <v>447221000</v>
       </c>
       <c r="K9">
-        <v>1000000</v>
+        <v>1281006000</v>
       </c>
       <c r="L9">
-        <v>10897000000</v>
+        <v>1728227000</v>
       </c>
       <c r="M9">
-        <v>1657000000</v>
+        <v>374963000</v>
       </c>
       <c r="N9">
-        <v>979000000</v>
+        <v>330674000</v>
       </c>
       <c r="O9">
-        <v>157000000</v>
+        <v>46966000</v>
       </c>
       <c r="P9">
-        <v>13690000000</v>
+        <v>2480830000</v>
       </c>
       <c r="Q9">
-        <v>2292000000</v>
+        <v>571858000</v>
       </c>
       <c r="R9">
-        <v>618000000</v>
+        <v>369844000</v>
       </c>
       <c r="S9">
-        <v>49000000</v>
+        <v>120458000</v>
       </c>
       <c r="T9">
-        <v>667000000</v>
+        <v>490302000</v>
       </c>
       <c r="U9">
-        <v>0</v>
+        <v>6630000</v>
       </c>
       <c r="V9">
-        <v>548000000</v>
+        <v>0</v>
       </c>
       <c r="W9">
-        <v>118000000</v>
+        <v>36298000</v>
       </c>
       <c r="X9">
-        <v>3625000000</v>
+        <v>1105088000</v>
       </c>
       <c r="Y9">
         <v>0</v>
       </c>
       <c r="Z9">
-        <v>17315000000</v>
+        <v>3585918000</v>
       </c>
       <c r="AA9">
-        <v>687000000</v>
+        <v>344527000</v>
       </c>
       <c r="AB9">
-        <v>91000000</v>
+        <v>0</v>
       </c>
       <c r="AC9">
-        <v>61000000</v>
+        <v>0</v>
       </c>
       <c r="AD9">
-        <v>141000000</v>
+        <v>19624000</v>
       </c>
       <c r="AE9">
-        <v>804000000</v>
+        <v>420227000</v>
       </c>
       <c r="AF9">
-        <v>1784000000</v>
+        <v>784378000</v>
       </c>
       <c r="AG9">
-        <v>2552000000</v>
+        <v>24450000</v>
       </c>
       <c r="AH9">
-        <v>60000000</v>
+        <v>0</v>
       </c>
       <c r="AI9">
-        <v>29000000</v>
+        <v>17739000</v>
       </c>
       <c r="AJ9">
-        <v>686000000</v>
+        <v>94211000</v>
       </c>
       <c r="AK9">
-        <v>3327000000</v>
+        <v>136400000</v>
       </c>
       <c r="AL9">
         <v>0</v>
       </c>
       <c r="AM9">
-        <v>652000000</v>
+        <v>24450000</v>
       </c>
       <c r="AN9">
-        <v>5111000000</v>
+        <v>920778000</v>
       </c>
       <c r="AO9">
         <v>0</v>
       </c>
       <c r="AP9">
-        <v>1000000</v>
+        <v>653000</v>
       </c>
       <c r="AQ9">
-        <v>14971000000</v>
+        <v>1896182000</v>
       </c>
       <c r="AR9">
-        <v>1000000</v>
+        <v>12172000</v>
       </c>
       <c r="AS9">
-        <v>-2769000000</v>
+        <v>756133000</v>
       </c>
       <c r="AT9">
-        <v>12204000000</v>
+        <v>2665140000</v>
       </c>
       <c r="AU9">
-        <v>12204000000</v>
+        <v>2665140000</v>
       </c>
       <c r="AV9">
-        <v>17315000000</v>
+        <v>3585918000</v>
       </c>
       <c r="AW9">
         <v>0</v>
       </c>
       <c r="AX9">
-        <v>17315000000</v>
+        <v>3585918000</v>
       </c>
       <c r="AY9">
-        <v>0</v>
+        <v>1287636000</v>
       </c>
       <c r="AZ9">
-        <v>2643000000</v>
+        <v>24450000</v>
       </c>
       <c r="BA9">
-        <v>-8253000000</v>
+        <v>-422771000</v>
       </c>
       <c r="BB9" s="3" t="s">
-        <v>106</v>
+        <v>143</v>
       </c>
       <c r="BC9" s="3" t="s">
-        <v>114</v>
+        <v>158</v>
       </c>
     </row>
     <row r="10" spans="1:55">
@@ -2253,166 +2388,166 @@
         <v>63</v>
       </c>
       <c r="B10" s="2">
-        <v>44227</v>
+        <v>40573</v>
       </c>
       <c r="C10" t="s">
-        <v>65</v>
+        <v>75</v>
       </c>
       <c r="D10" t="s">
-        <v>66</v>
+        <v>76</v>
       </c>
       <c r="E10" t="s">
-        <v>67</v>
+        <v>77</v>
       </c>
       <c r="F10" t="s">
-        <v>76</v>
+        <v>86</v>
       </c>
       <c r="G10" t="s">
-        <v>86</v>
+        <v>106</v>
       </c>
       <c r="H10" t="s">
-        <v>96</v>
+        <v>126</v>
       </c>
       <c r="I10" t="s">
-        <v>98</v>
+        <v>138</v>
       </c>
       <c r="J10">
-        <v>847000000</v>
+        <v>665361000</v>
       </c>
       <c r="K10">
-        <v>10714000000</v>
+        <v>1825202000</v>
       </c>
       <c r="L10">
-        <v>11561000000</v>
+        <v>2490563000</v>
       </c>
       <c r="M10">
-        <v>2429000000</v>
+        <v>348770000</v>
       </c>
       <c r="N10">
-        <v>1826000000</v>
+        <v>345525000</v>
       </c>
       <c r="O10">
-        <v>239000000</v>
+        <v>42092000</v>
       </c>
       <c r="P10">
-        <v>16055000000</v>
+        <v>3226950000</v>
       </c>
       <c r="Q10">
-        <v>2856000000</v>
+        <v>568857000</v>
       </c>
       <c r="R10">
-        <v>4193000000</v>
+        <v>369844000</v>
       </c>
       <c r="S10">
-        <v>2737000000</v>
+        <v>288745000</v>
       </c>
       <c r="T10">
-        <v>6930000000</v>
+        <v>658589000</v>
       </c>
       <c r="U10">
-        <v>144000000</v>
+        <v>8792000</v>
       </c>
       <c r="V10">
-        <v>806000000</v>
+        <v>0</v>
       </c>
       <c r="W10">
-        <v>2000000000</v>
+        <v>32058000</v>
       </c>
       <c r="X10">
-        <v>12736000000</v>
+        <v>1268296000</v>
       </c>
       <c r="Y10">
         <v>0</v>
       </c>
       <c r="Z10">
-        <v>28791000000</v>
+        <v>4495246000</v>
       </c>
       <c r="AA10">
-        <v>1201000000</v>
+        <v>286138000</v>
       </c>
       <c r="AB10">
-        <v>1120000000</v>
+        <v>0</v>
       </c>
       <c r="AC10">
-        <v>61000000</v>
+        <v>4576000</v>
       </c>
       <c r="AD10">
-        <v>288000000</v>
+        <v>248864000</v>
       </c>
       <c r="AE10">
-        <v>1255000000</v>
+        <v>403104000</v>
       </c>
       <c r="AF10">
-        <v>3925000000</v>
+        <v>942682000</v>
       </c>
       <c r="AG10">
-        <v>6598000000</v>
+        <v>23389000</v>
       </c>
       <c r="AH10">
         <v>163000000</v>
       </c>
       <c r="AI10">
-        <v>241000000</v>
+        <v>46129000</v>
       </c>
       <c r="AJ10">
-        <v>971000000</v>
+        <v>138584000</v>
       </c>
       <c r="AK10">
-        <v>7973000000</v>
+        <v>371102000</v>
       </c>
       <c r="AL10">
         <v>0</v>
       </c>
       <c r="AM10">
-        <v>755000000</v>
+        <v>23389000</v>
       </c>
       <c r="AN10">
-        <v>11898000000</v>
+        <v>1313784000</v>
       </c>
       <c r="AO10">
         <v>0</v>
       </c>
       <c r="AP10">
-        <v>1000000</v>
+        <v>677000</v>
       </c>
       <c r="AQ10">
-        <v>18908000000</v>
+        <v>2149328000</v>
       </c>
       <c r="AR10">
-        <v>19000000</v>
+        <v>10272000</v>
       </c>
       <c r="AS10">
-        <v>-2035000000</v>
+        <v>1021185000</v>
       </c>
       <c r="AT10">
-        <v>16893000000</v>
+        <v>3181462000</v>
       </c>
       <c r="AU10">
-        <v>16893000000</v>
+        <v>3181462000</v>
       </c>
       <c r="AV10">
-        <v>28791000000</v>
+        <v>4495246000</v>
       </c>
       <c r="AW10">
         <v>0</v>
       </c>
       <c r="AX10">
-        <v>28791000000</v>
+        <v>4495246000</v>
       </c>
       <c r="AY10">
-        <v>10858000000</v>
+        <v>1833994000</v>
       </c>
       <c r="AZ10">
-        <v>7718000000</v>
+        <v>23389000</v>
       </c>
       <c r="BA10">
-        <v>6871000000</v>
+        <v>-641972000</v>
       </c>
       <c r="BB10" s="3" t="s">
-        <v>107</v>
+        <v>144</v>
       </c>
       <c r="BC10" s="3" t="s">
-        <v>115</v>
+        <v>144</v>
       </c>
     </row>
     <row r="11" spans="1:55">
@@ -2420,190 +2555,1874 @@
         <v>64</v>
       </c>
       <c r="B11" s="2">
+        <v>40937</v>
+      </c>
+      <c r="C11" t="s">
+        <v>75</v>
+      </c>
+      <c r="D11" t="s">
+        <v>76</v>
+      </c>
+      <c r="E11" t="s">
+        <v>77</v>
+      </c>
+      <c r="F11" t="s">
+        <v>87</v>
+      </c>
+      <c r="G11" t="s">
+        <v>107</v>
+      </c>
+      <c r="H11" t="s">
+        <v>127</v>
+      </c>
+      <c r="I11" t="s">
+        <v>138</v>
+      </c>
+      <c r="J11">
+        <v>667876000</v>
+      </c>
+      <c r="K11">
+        <v>2461700000</v>
+      </c>
+      <c r="L11">
+        <v>3129576000</v>
+      </c>
+      <c r="M11">
+        <v>336143000</v>
+      </c>
+      <c r="N11">
+        <v>340297000</v>
+      </c>
+      <c r="O11">
+        <v>99342000</v>
+      </c>
+      <c r="P11">
+        <v>3905358000</v>
+      </c>
+      <c r="Q11">
+        <v>560072000</v>
+      </c>
+      <c r="R11">
+        <v>641030000</v>
+      </c>
+      <c r="S11">
+        <v>326136000</v>
+      </c>
+      <c r="T11">
+        <v>967166000</v>
+      </c>
+      <c r="U11">
+        <v>10382000</v>
+      </c>
+      <c r="V11">
+        <v>7459000</v>
+      </c>
+      <c r="W11">
+        <v>102491000</v>
+      </c>
+      <c r="X11">
+        <v>1647570000</v>
+      </c>
+      <c r="Y11">
+        <v>0</v>
+      </c>
+      <c r="Z11">
+        <v>5552928000</v>
+      </c>
+      <c r="AA11">
+        <v>335072000</v>
+      </c>
+      <c r="AB11">
+        <v>0</v>
+      </c>
+      <c r="AC11">
+        <v>6941000</v>
+      </c>
+      <c r="AD11">
+        <v>270649000</v>
+      </c>
+      <c r="AE11">
+        <v>317296000</v>
+      </c>
+      <c r="AF11">
+        <v>929958000</v>
+      </c>
+      <c r="AG11">
+        <v>21439000</v>
+      </c>
+      <c r="AH11">
+        <v>200370000</v>
+      </c>
+      <c r="AI11">
+        <v>133288000</v>
+      </c>
+      <c r="AJ11">
+        <v>122149000</v>
+      </c>
+      <c r="AK11">
+        <v>477246000</v>
+      </c>
+      <c r="AL11">
+        <v>0</v>
+      </c>
+      <c r="AM11">
+        <v>21439000</v>
+      </c>
+      <c r="AN11">
+        <v>1407204000</v>
+      </c>
+      <c r="AO11">
+        <v>0</v>
+      </c>
+      <c r="AP11">
+        <v>700000</v>
+      </c>
+      <c r="AQ11">
+        <v>2730418000</v>
+      </c>
+      <c r="AR11">
+        <v>10614000</v>
+      </c>
+      <c r="AS11">
+        <v>1403992000</v>
+      </c>
+      <c r="AT11">
+        <v>4145724000</v>
+      </c>
+      <c r="AU11">
+        <v>4145724000</v>
+      </c>
+      <c r="AV11">
+        <v>5552928000</v>
+      </c>
+      <c r="AW11">
+        <v>0</v>
+      </c>
+      <c r="AX11">
+        <v>5552928000</v>
+      </c>
+      <c r="AY11">
+        <v>2472082000</v>
+      </c>
+      <c r="AZ11">
+        <v>21439000</v>
+      </c>
+      <c r="BA11">
+        <v>-646437000</v>
+      </c>
+      <c r="BB11" s="3" t="s">
+        <v>145</v>
+      </c>
+      <c r="BC11" s="3" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="12" spans="1:55">
+      <c r="A12" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="B12" s="2">
+        <v>41301</v>
+      </c>
+      <c r="C12" t="s">
+        <v>75</v>
+      </c>
+      <c r="D12" t="s">
+        <v>76</v>
+      </c>
+      <c r="E12" t="s">
+        <v>77</v>
+      </c>
+      <c r="F12" t="s">
+        <v>88</v>
+      </c>
+      <c r="G12" t="s">
+        <v>108</v>
+      </c>
+      <c r="H12" t="s">
+        <v>128</v>
+      </c>
+      <c r="I12" t="s">
+        <v>138</v>
+      </c>
+      <c r="J12">
+        <v>732786000</v>
+      </c>
+      <c r="K12">
+        <v>2995097000</v>
+      </c>
+      <c r="L12">
+        <v>3727883000</v>
+      </c>
+      <c r="M12">
+        <v>454252000</v>
+      </c>
+      <c r="N12">
+        <v>419686000</v>
+      </c>
+      <c r="O12">
+        <v>173437000</v>
+      </c>
+      <c r="P12">
+        <v>4775258000</v>
+      </c>
+      <c r="Q12">
+        <v>576144000</v>
+      </c>
+      <c r="R12">
+        <v>641030000</v>
+      </c>
+      <c r="S12">
+        <v>312332000</v>
+      </c>
+      <c r="T12">
+        <v>953362000</v>
+      </c>
+      <c r="U12">
+        <v>10030000</v>
+      </c>
+      <c r="V12">
+        <v>3527000</v>
+      </c>
+      <c r="W12">
+        <v>93924000</v>
+      </c>
+      <c r="X12">
+        <v>1636987000</v>
+      </c>
+      <c r="Y12">
+        <v>0</v>
+      </c>
+      <c r="Z12">
+        <v>6412245000</v>
+      </c>
+      <c r="AA12">
+        <v>356428000</v>
+      </c>
+      <c r="AB12">
+        <v>0</v>
+      </c>
+      <c r="AC12">
+        <v>3173000</v>
+      </c>
+      <c r="AD12">
+        <v>273605000</v>
+      </c>
+      <c r="AE12">
+        <v>343017000</v>
+      </c>
+      <c r="AF12">
+        <v>976223000</v>
+      </c>
+      <c r="AG12">
+        <v>18998000</v>
+      </c>
+      <c r="AH12">
+        <v>236152000</v>
+      </c>
+      <c r="AI12">
+        <v>192950000</v>
+      </c>
+      <c r="AJ12">
+        <v>160219000</v>
+      </c>
+      <c r="AK12">
+        <v>608319000</v>
+      </c>
+      <c r="AL12">
+        <v>0</v>
+      </c>
+      <c r="AM12">
+        <v>18998000</v>
+      </c>
+      <c r="AN12">
+        <v>1584542000</v>
+      </c>
+      <c r="AO12">
+        <v>0</v>
+      </c>
+      <c r="AP12">
+        <v>720000</v>
+      </c>
+      <c r="AQ12">
+        <v>3246088000</v>
+      </c>
+      <c r="AR12">
+        <v>9981000</v>
+      </c>
+      <c r="AS12">
+        <v>1570914000</v>
+      </c>
+      <c r="AT12">
+        <v>4827703000</v>
+      </c>
+      <c r="AU12">
+        <v>4827703000</v>
+      </c>
+      <c r="AV12">
+        <v>6412245000</v>
+      </c>
+      <c r="AW12">
+        <v>0</v>
+      </c>
+      <c r="AX12">
+        <v>6412245000</v>
+      </c>
+      <c r="AY12">
+        <v>3005127000</v>
+      </c>
+      <c r="AZ12">
+        <v>18998000</v>
+      </c>
+      <c r="BA12">
+        <v>-713788000</v>
+      </c>
+      <c r="BB12" s="3" t="s">
+        <v>146</v>
+      </c>
+      <c r="BC12" s="3" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="13" spans="1:55">
+      <c r="A13" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="B13" s="2">
+        <v>41665</v>
+      </c>
+      <c r="C13" t="s">
+        <v>75</v>
+      </c>
+      <c r="D13" t="s">
+        <v>76</v>
+      </c>
+      <c r="E13" t="s">
+        <v>77</v>
+      </c>
+      <c r="F13" t="s">
+        <v>89</v>
+      </c>
+      <c r="G13" t="s">
+        <v>109</v>
+      </c>
+      <c r="H13" t="s">
+        <v>129</v>
+      </c>
+      <c r="I13" t="s">
+        <v>138</v>
+      </c>
+      <c r="J13">
+        <v>1151587000</v>
+      </c>
+      <c r="K13">
+        <v>3520223000</v>
+      </c>
+      <c r="L13">
+        <v>4671810000</v>
+      </c>
+      <c r="M13">
+        <v>426357000</v>
+      </c>
+      <c r="N13">
+        <v>387765000</v>
+      </c>
+      <c r="O13">
+        <v>138779000</v>
+      </c>
+      <c r="P13">
+        <v>5624711000</v>
+      </c>
+      <c r="Q13">
+        <v>582740000</v>
+      </c>
+      <c r="R13">
+        <v>643179000</v>
+      </c>
+      <c r="S13">
+        <v>296012000</v>
+      </c>
+      <c r="T13">
+        <v>939191000</v>
+      </c>
+      <c r="U13">
+        <v>0</v>
+      </c>
+      <c r="V13">
+        <v>0</v>
+      </c>
+      <c r="W13">
+        <v>104252000</v>
+      </c>
+      <c r="X13">
+        <v>1626183000</v>
+      </c>
+      <c r="Y13">
+        <v>0</v>
+      </c>
+      <c r="Z13">
+        <v>7250894000</v>
+      </c>
+      <c r="AA13">
+        <v>324391000</v>
+      </c>
+      <c r="AB13">
+        <v>0</v>
+      </c>
+      <c r="AC13">
+        <v>2378000</v>
+      </c>
+      <c r="AD13">
+        <v>282405000</v>
+      </c>
+      <c r="AE13">
+        <v>336322000</v>
+      </c>
+      <c r="AF13">
+        <v>945496000</v>
+      </c>
+      <c r="AG13">
+        <v>1373875000</v>
+      </c>
+      <c r="AH13">
+        <v>172199000</v>
+      </c>
+      <c r="AI13">
+        <v>157953000</v>
+      </c>
+      <c r="AJ13">
+        <v>144973000</v>
+      </c>
+      <c r="AK13">
+        <v>1849000000</v>
+      </c>
+      <c r="AL13">
+        <v>0</v>
+      </c>
+      <c r="AM13">
+        <v>17500000</v>
+      </c>
+      <c r="AN13">
+        <v>2794496000</v>
+      </c>
+      <c r="AO13">
+        <v>0</v>
+      </c>
+      <c r="AP13">
+        <v>732000</v>
+      </c>
+      <c r="AQ13">
+        <v>3504742000</v>
+      </c>
+      <c r="AR13">
+        <v>4877000</v>
+      </c>
+      <c r="AS13">
+        <v>946047000</v>
+      </c>
+      <c r="AT13">
+        <v>4456398000</v>
+      </c>
+      <c r="AU13">
+        <v>4456398000</v>
+      </c>
+      <c r="AV13">
+        <v>7250894000</v>
+      </c>
+      <c r="AW13">
+        <v>0</v>
+      </c>
+      <c r="AX13">
+        <v>7250894000</v>
+      </c>
+      <c r="AY13">
+        <v>0</v>
+      </c>
+      <c r="AZ13">
+        <v>1373875000</v>
+      </c>
+      <c r="BA13">
+        <v>222288000</v>
+      </c>
+      <c r="BB13" s="3" t="s">
+        <v>147</v>
+      </c>
+      <c r="BC13" s="3" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="14" spans="1:55">
+      <c r="A14" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="B14" s="2">
+        <v>42029</v>
+      </c>
+      <c r="C14" t="s">
+        <v>75</v>
+      </c>
+      <c r="D14" t="s">
+        <v>76</v>
+      </c>
+      <c r="E14" t="s">
+        <v>77</v>
+      </c>
+      <c r="F14" t="s">
+        <v>90</v>
+      </c>
+      <c r="G14" t="s">
+        <v>110</v>
+      </c>
+      <c r="H14" t="s">
+        <v>130</v>
+      </c>
+      <c r="I14" t="s">
+        <v>138</v>
+      </c>
+      <c r="J14">
+        <v>496654000</v>
+      </c>
+      <c r="K14">
+        <v>4126685000</v>
+      </c>
+      <c r="L14">
+        <v>4623339000</v>
+      </c>
+      <c r="M14">
+        <v>473637000</v>
+      </c>
+      <c r="N14">
+        <v>482893000</v>
+      </c>
+      <c r="O14">
+        <v>133428000</v>
+      </c>
+      <c r="P14">
+        <v>5713297000</v>
+      </c>
+      <c r="Q14">
+        <v>557282000</v>
+      </c>
+      <c r="R14">
+        <v>618179000</v>
+      </c>
+      <c r="S14">
+        <v>221714000</v>
+      </c>
+      <c r="T14">
+        <v>839893000</v>
+      </c>
+      <c r="U14">
+        <v>0</v>
+      </c>
+      <c r="V14">
+        <v>0</v>
+      </c>
+      <c r="W14">
+        <v>90896000</v>
+      </c>
+      <c r="X14">
+        <v>1488071000</v>
+      </c>
+      <c r="Y14">
+        <v>0</v>
+      </c>
+      <c r="Z14">
+        <v>7201368000</v>
+      </c>
+      <c r="AA14">
+        <v>293223000</v>
+      </c>
+      <c r="AB14">
+        <v>0</v>
+      </c>
+      <c r="AC14">
+        <v>2810000</v>
+      </c>
+      <c r="AD14">
+        <v>292735000</v>
+      </c>
+      <c r="AE14">
+        <v>307262000</v>
+      </c>
+      <c r="AF14">
+        <v>896030000</v>
+      </c>
+      <c r="AG14">
+        <v>1398428000</v>
+      </c>
+      <c r="AH14">
+        <v>107838000</v>
+      </c>
+      <c r="AI14">
+        <v>232307000</v>
+      </c>
+      <c r="AJ14">
+        <v>148783000</v>
+      </c>
+      <c r="AK14">
+        <v>1887356000</v>
+      </c>
+      <c r="AL14">
+        <v>0</v>
+      </c>
+      <c r="AM14">
+        <v>14086000</v>
+      </c>
+      <c r="AN14">
+        <v>2783386000</v>
+      </c>
+      <c r="AO14">
+        <v>0</v>
+      </c>
+      <c r="AP14">
+        <v>754000</v>
+      </c>
+      <c r="AQ14">
+        <v>3948877000</v>
+      </c>
+      <c r="AR14">
+        <v>7844000</v>
+      </c>
+      <c r="AS14">
+        <v>460507000</v>
+      </c>
+      <c r="AT14">
+        <v>4417982000</v>
+      </c>
+      <c r="AU14">
+        <v>4417982000</v>
+      </c>
+      <c r="AV14">
+        <v>7201368000</v>
+      </c>
+      <c r="AW14">
+        <v>0</v>
+      </c>
+      <c r="AX14">
+        <v>7201368000</v>
+      </c>
+      <c r="AY14">
+        <v>0</v>
+      </c>
+      <c r="AZ14">
+        <v>1398428000</v>
+      </c>
+      <c r="BA14">
+        <v>901774000</v>
+      </c>
+      <c r="BB14" s="3" t="s">
+        <v>148</v>
+      </c>
+      <c r="BC14" s="3" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="15" spans="1:55">
+      <c r="A15" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="B15" s="2">
+        <v>42400</v>
+      </c>
+      <c r="C15" t="s">
+        <v>75</v>
+      </c>
+      <c r="D15" t="s">
+        <v>76</v>
+      </c>
+      <c r="E15" t="s">
+        <v>77</v>
+      </c>
+      <c r="F15" t="s">
+        <v>91</v>
+      </c>
+      <c r="G15" t="s">
+        <v>111</v>
+      </c>
+      <c r="H15" t="s">
+        <v>131</v>
+      </c>
+      <c r="I15" t="s">
+        <v>138</v>
+      </c>
+      <c r="J15">
+        <v>596000000</v>
+      </c>
+      <c r="K15">
+        <v>4441000000</v>
+      </c>
+      <c r="L15">
+        <v>5037000000</v>
+      </c>
+      <c r="M15">
+        <v>505000000</v>
+      </c>
+      <c r="N15">
+        <v>418000000</v>
+      </c>
+      <c r="O15">
+        <v>93000000</v>
+      </c>
+      <c r="P15">
+        <v>6053000000</v>
+      </c>
+      <c r="Q15">
+        <v>466000000</v>
+      </c>
+      <c r="R15">
+        <v>618000000</v>
+      </c>
+      <c r="S15">
+        <v>166000000</v>
+      </c>
+      <c r="T15">
+        <v>784000000</v>
+      </c>
+      <c r="U15">
+        <v>0</v>
+      </c>
+      <c r="V15">
+        <v>0</v>
+      </c>
+      <c r="W15">
+        <v>67000000</v>
+      </c>
+      <c r="X15">
+        <v>1317000000</v>
+      </c>
+      <c r="Y15">
+        <v>0</v>
+      </c>
+      <c r="Z15">
+        <v>7370000000</v>
+      </c>
+      <c r="AA15">
+        <v>296000000</v>
+      </c>
+      <c r="AB15">
+        <v>1500000000</v>
+      </c>
+      <c r="AC15">
+        <v>2000000</v>
+      </c>
+      <c r="AD15">
+        <v>322000000</v>
+      </c>
+      <c r="AE15">
+        <v>318000000</v>
+      </c>
+      <c r="AF15">
+        <v>2438000000</v>
+      </c>
+      <c r="AG15">
+        <v>10000000</v>
+      </c>
+      <c r="AH15">
+        <v>44000000</v>
+      </c>
+      <c r="AI15">
+        <v>301000000</v>
+      </c>
+      <c r="AJ15">
+        <v>108000000</v>
+      </c>
+      <c r="AK15">
+        <v>463000000</v>
+      </c>
+      <c r="AL15">
+        <v>0</v>
+      </c>
+      <c r="AM15">
+        <v>10000000</v>
+      </c>
+      <c r="AN15">
+        <v>2901000000</v>
+      </c>
+      <c r="AO15">
+        <v>0</v>
+      </c>
+      <c r="AP15">
+        <v>1000000</v>
+      </c>
+      <c r="AQ15">
+        <v>4350000000</v>
+      </c>
+      <c r="AR15">
+        <v>-4000000</v>
+      </c>
+      <c r="AS15">
+        <v>122000000</v>
+      </c>
+      <c r="AT15">
+        <v>4469000000</v>
+      </c>
+      <c r="AU15">
+        <v>4469000000</v>
+      </c>
+      <c r="AV15">
+        <v>7370000000</v>
+      </c>
+      <c r="AW15">
+        <v>0</v>
+      </c>
+      <c r="AX15">
+        <v>7370000000</v>
+      </c>
+      <c r="AY15">
+        <v>0</v>
+      </c>
+      <c r="AZ15">
+        <v>1510000000</v>
+      </c>
+      <c r="BA15">
+        <v>914000000</v>
+      </c>
+      <c r="BB15" s="3" t="s">
+        <v>149</v>
+      </c>
+      <c r="BC15" s="3" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="16" spans="1:55">
+      <c r="A16" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="B16" s="2">
+        <v>42764</v>
+      </c>
+      <c r="C16" t="s">
+        <v>75</v>
+      </c>
+      <c r="D16" t="s">
+        <v>76</v>
+      </c>
+      <c r="E16" t="s">
+        <v>77</v>
+      </c>
+      <c r="F16" t="s">
+        <v>92</v>
+      </c>
+      <c r="G16" t="s">
+        <v>112</v>
+      </c>
+      <c r="H16" t="s">
+        <v>132</v>
+      </c>
+      <c r="I16" t="s">
+        <v>138</v>
+      </c>
+      <c r="J16">
+        <v>1766000000</v>
+      </c>
+      <c r="K16">
+        <v>5032000000</v>
+      </c>
+      <c r="L16">
+        <v>6798000000</v>
+      </c>
+      <c r="M16">
+        <v>826000000</v>
+      </c>
+      <c r="N16">
+        <v>794000000</v>
+      </c>
+      <c r="O16">
+        <v>118000000</v>
+      </c>
+      <c r="P16">
+        <v>8536000000</v>
+      </c>
+      <c r="Q16">
+        <v>521000000</v>
+      </c>
+      <c r="R16">
+        <v>618000000</v>
+      </c>
+      <c r="S16">
+        <v>104000000</v>
+      </c>
+      <c r="T16">
+        <v>722000000</v>
+      </c>
+      <c r="U16">
+        <v>0</v>
+      </c>
+      <c r="V16">
+        <v>0</v>
+      </c>
+      <c r="W16">
+        <v>62000000</v>
+      </c>
+      <c r="X16">
+        <v>1305000000</v>
+      </c>
+      <c r="Y16">
+        <v>0</v>
+      </c>
+      <c r="Z16">
+        <v>9841000000</v>
+      </c>
+      <c r="AA16">
+        <v>485000000</v>
+      </c>
+      <c r="AB16">
+        <v>827000000</v>
+      </c>
+      <c r="AC16">
+        <v>4000000</v>
+      </c>
+      <c r="AD16">
+        <v>85000000</v>
+      </c>
+      <c r="AE16">
+        <v>418000000</v>
+      </c>
+      <c r="AF16">
+        <v>1819000000</v>
+      </c>
+      <c r="AG16">
+        <v>1989000000</v>
+      </c>
+      <c r="AH16">
+        <v>4000000</v>
+      </c>
+      <c r="AI16">
+        <v>141000000</v>
+      </c>
+      <c r="AJ16">
+        <v>126000000</v>
+      </c>
+      <c r="AK16">
+        <v>2260000000</v>
+      </c>
+      <c r="AL16">
+        <v>0</v>
+      </c>
+      <c r="AM16">
+        <v>6000000</v>
+      </c>
+      <c r="AN16">
+        <v>4079000000</v>
+      </c>
+      <c r="AO16">
+        <v>0</v>
+      </c>
+      <c r="AP16">
+        <v>1000000</v>
+      </c>
+      <c r="AQ16">
+        <v>6108000000</v>
+      </c>
+      <c r="AR16">
+        <v>-16000000</v>
+      </c>
+      <c r="AS16">
+        <v>-331000000</v>
+      </c>
+      <c r="AT16">
+        <v>5762000000</v>
+      </c>
+      <c r="AU16">
+        <v>5762000000</v>
+      </c>
+      <c r="AV16">
+        <v>9841000000</v>
+      </c>
+      <c r="AW16">
+        <v>0</v>
+      </c>
+      <c r="AX16">
+        <v>9841000000</v>
+      </c>
+      <c r="AY16">
+        <v>0</v>
+      </c>
+      <c r="AZ16">
+        <v>2816000000</v>
+      </c>
+      <c r="BA16">
+        <v>1050000000</v>
+      </c>
+      <c r="BB16" s="3" t="s">
+        <v>150</v>
+      </c>
+      <c r="BC16" s="3" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="17" spans="1:55">
+      <c r="A17" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="B17" s="2">
+        <v>43128</v>
+      </c>
+      <c r="C17" t="s">
+        <v>75</v>
+      </c>
+      <c r="D17" t="s">
+        <v>76</v>
+      </c>
+      <c r="E17" t="s">
+        <v>77</v>
+      </c>
+      <c r="F17" t="s">
+        <v>93</v>
+      </c>
+      <c r="G17" t="s">
+        <v>113</v>
+      </c>
+      <c r="H17" t="s">
+        <v>133</v>
+      </c>
+      <c r="I17" t="s">
+        <v>138</v>
+      </c>
+      <c r="J17">
+        <v>4002000000</v>
+      </c>
+      <c r="K17">
+        <v>3106000000</v>
+      </c>
+      <c r="L17">
+        <v>7108000000</v>
+      </c>
+      <c r="M17">
+        <v>1265000000</v>
+      </c>
+      <c r="N17">
+        <v>796000000</v>
+      </c>
+      <c r="O17">
+        <v>86000000</v>
+      </c>
+      <c r="P17">
+        <v>9255000000</v>
+      </c>
+      <c r="Q17">
+        <v>997000000</v>
+      </c>
+      <c r="R17">
+        <v>618000000</v>
+      </c>
+      <c r="S17">
+        <v>52000000</v>
+      </c>
+      <c r="T17">
+        <v>670000000</v>
+      </c>
+      <c r="U17">
+        <v>0</v>
+      </c>
+      <c r="V17">
+        <v>0</v>
+      </c>
+      <c r="W17">
+        <v>319000000</v>
+      </c>
+      <c r="X17">
+        <v>1986000000</v>
+      </c>
+      <c r="Y17">
+        <v>0</v>
+      </c>
+      <c r="Z17">
+        <v>11241000000</v>
+      </c>
+      <c r="AA17">
+        <v>596000000</v>
+      </c>
+      <c r="AB17">
+        <v>15000000</v>
+      </c>
+      <c r="AC17">
+        <v>33000000</v>
+      </c>
+      <c r="AD17">
+        <v>53000000</v>
+      </c>
+      <c r="AE17">
+        <v>456000000</v>
+      </c>
+      <c r="AF17">
+        <v>1153000000</v>
+      </c>
+      <c r="AG17">
+        <v>1985000000</v>
+      </c>
+      <c r="AH17">
+        <v>15000000</v>
+      </c>
+      <c r="AI17">
+        <v>18000000</v>
+      </c>
+      <c r="AJ17">
+        <v>599000000</v>
+      </c>
+      <c r="AK17">
+        <v>2617000000</v>
+      </c>
+      <c r="AL17">
+        <v>0</v>
+      </c>
+      <c r="AM17">
+        <v>0</v>
+      </c>
+      <c r="AN17">
+        <v>3770000000</v>
+      </c>
+      <c r="AO17">
+        <v>0</v>
+      </c>
+      <c r="AP17">
+        <v>1000000</v>
+      </c>
+      <c r="AQ17">
+        <v>8787000000</v>
+      </c>
+      <c r="AR17">
+        <v>-18000000</v>
+      </c>
+      <c r="AS17">
+        <v>-1299000000</v>
+      </c>
+      <c r="AT17">
+        <v>7471000000</v>
+      </c>
+      <c r="AU17">
+        <v>7471000000</v>
+      </c>
+      <c r="AV17">
+        <v>11241000000</v>
+      </c>
+      <c r="AW17">
+        <v>0</v>
+      </c>
+      <c r="AX17">
+        <v>11241000000</v>
+      </c>
+      <c r="AY17">
+        <v>0</v>
+      </c>
+      <c r="AZ17">
+        <v>2000000000</v>
+      </c>
+      <c r="BA17">
+        <v>-2002000000</v>
+      </c>
+      <c r="BB17" s="3" t="s">
+        <v>151</v>
+      </c>
+      <c r="BC17" s="3" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="18" spans="1:55">
+      <c r="A18" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="B18" s="2">
+        <v>43492</v>
+      </c>
+      <c r="C18" t="s">
+        <v>75</v>
+      </c>
+      <c r="D18" t="s">
+        <v>76</v>
+      </c>
+      <c r="E18" t="s">
+        <v>77</v>
+      </c>
+      <c r="F18" t="s">
+        <v>94</v>
+      </c>
+      <c r="G18" t="s">
+        <v>114</v>
+      </c>
+      <c r="H18" t="s">
+        <v>134</v>
+      </c>
+      <c r="I18" t="s">
+        <v>138</v>
+      </c>
+      <c r="J18">
+        <v>782000000</v>
+      </c>
+      <c r="K18">
+        <v>6640000000</v>
+      </c>
+      <c r="L18">
+        <v>7422000000</v>
+      </c>
+      <c r="M18">
+        <v>1424000000</v>
+      </c>
+      <c r="N18">
+        <v>1575000000</v>
+      </c>
+      <c r="O18">
+        <v>136000000</v>
+      </c>
+      <c r="P18">
+        <v>10557000000</v>
+      </c>
+      <c r="Q18">
+        <v>1404000000</v>
+      </c>
+      <c r="R18">
+        <v>618000000</v>
+      </c>
+      <c r="S18">
+        <v>45000000</v>
+      </c>
+      <c r="T18">
+        <v>663000000</v>
+      </c>
+      <c r="U18">
+        <v>0</v>
+      </c>
+      <c r="V18">
+        <v>0</v>
+      </c>
+      <c r="W18">
+        <v>668000000</v>
+      </c>
+      <c r="X18">
+        <v>2735000000</v>
+      </c>
+      <c r="Y18">
+        <v>0</v>
+      </c>
+      <c r="Z18">
+        <v>13292000000</v>
+      </c>
+      <c r="AA18">
+        <v>511000000</v>
+      </c>
+      <c r="AB18">
+        <v>0</v>
+      </c>
+      <c r="AC18">
+        <v>91000000</v>
+      </c>
+      <c r="AD18">
+        <v>92000000</v>
+      </c>
+      <c r="AE18">
+        <v>635000000</v>
+      </c>
+      <c r="AF18">
+        <v>1329000000</v>
+      </c>
+      <c r="AG18">
+        <v>1988000000</v>
+      </c>
+      <c r="AH18">
+        <v>46000000</v>
+      </c>
+      <c r="AI18">
+        <v>19000000</v>
+      </c>
+      <c r="AJ18">
+        <v>568000000</v>
+      </c>
+      <c r="AK18">
+        <v>2621000000</v>
+      </c>
+      <c r="AL18">
+        <v>0</v>
+      </c>
+      <c r="AM18">
+        <v>0</v>
+      </c>
+      <c r="AN18">
+        <v>3950000000</v>
+      </c>
+      <c r="AO18">
+        <v>0</v>
+      </c>
+      <c r="AP18">
+        <v>1000000</v>
+      </c>
+      <c r="AQ18">
+        <v>12565000000</v>
+      </c>
+      <c r="AR18">
+        <v>-12000000</v>
+      </c>
+      <c r="AS18">
+        <v>-3212000000</v>
+      </c>
+      <c r="AT18">
+        <v>9342000000</v>
+      </c>
+      <c r="AU18">
+        <v>9342000000</v>
+      </c>
+      <c r="AV18">
+        <v>13292000000</v>
+      </c>
+      <c r="AW18">
+        <v>0</v>
+      </c>
+      <c r="AX18">
+        <v>13292000000</v>
+      </c>
+      <c r="AY18">
+        <v>0</v>
+      </c>
+      <c r="AZ18">
+        <v>1988000000</v>
+      </c>
+      <c r="BA18">
+        <v>1206000000</v>
+      </c>
+      <c r="BB18" s="3" t="s">
+        <v>152</v>
+      </c>
+      <c r="BC18" s="3" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="19" spans="1:55">
+      <c r="A19" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="B19" s="2">
+        <v>43856</v>
+      </c>
+      <c r="C19" t="s">
+        <v>75</v>
+      </c>
+      <c r="D19" t="s">
+        <v>76</v>
+      </c>
+      <c r="E19" t="s">
+        <v>77</v>
+      </c>
+      <c r="F19" t="s">
+        <v>95</v>
+      </c>
+      <c r="G19" t="s">
+        <v>115</v>
+      </c>
+      <c r="H19" t="s">
+        <v>135</v>
+      </c>
+      <c r="I19" t="s">
+        <v>138</v>
+      </c>
+      <c r="J19">
+        <v>10896000000</v>
+      </c>
+      <c r="K19">
+        <v>1000000</v>
+      </c>
+      <c r="L19">
+        <v>10897000000</v>
+      </c>
+      <c r="M19">
+        <v>1657000000</v>
+      </c>
+      <c r="N19">
+        <v>979000000</v>
+      </c>
+      <c r="O19">
+        <v>157000000</v>
+      </c>
+      <c r="P19">
+        <v>13690000000</v>
+      </c>
+      <c r="Q19">
+        <v>2292000000</v>
+      </c>
+      <c r="R19">
+        <v>618000000</v>
+      </c>
+      <c r="S19">
+        <v>49000000</v>
+      </c>
+      <c r="T19">
+        <v>667000000</v>
+      </c>
+      <c r="U19">
+        <v>0</v>
+      </c>
+      <c r="V19">
+        <v>548000000</v>
+      </c>
+      <c r="W19">
+        <v>118000000</v>
+      </c>
+      <c r="X19">
+        <v>3625000000</v>
+      </c>
+      <c r="Y19">
+        <v>0</v>
+      </c>
+      <c r="Z19">
+        <v>17315000000</v>
+      </c>
+      <c r="AA19">
+        <v>687000000</v>
+      </c>
+      <c r="AB19">
+        <v>91000000</v>
+      </c>
+      <c r="AC19">
+        <v>61000000</v>
+      </c>
+      <c r="AD19">
+        <v>141000000</v>
+      </c>
+      <c r="AE19">
+        <v>804000000</v>
+      </c>
+      <c r="AF19">
+        <v>1784000000</v>
+      </c>
+      <c r="AG19">
+        <v>2552000000</v>
+      </c>
+      <c r="AH19">
+        <v>60000000</v>
+      </c>
+      <c r="AI19">
+        <v>29000000</v>
+      </c>
+      <c r="AJ19">
+        <v>686000000</v>
+      </c>
+      <c r="AK19">
+        <v>3327000000</v>
+      </c>
+      <c r="AL19">
+        <v>0</v>
+      </c>
+      <c r="AM19">
+        <v>652000000</v>
+      </c>
+      <c r="AN19">
+        <v>5111000000</v>
+      </c>
+      <c r="AO19">
+        <v>0</v>
+      </c>
+      <c r="AP19">
+        <v>1000000</v>
+      </c>
+      <c r="AQ19">
+        <v>14971000000</v>
+      </c>
+      <c r="AR19">
+        <v>1000000</v>
+      </c>
+      <c r="AS19">
+        <v>-2769000000</v>
+      </c>
+      <c r="AT19">
+        <v>12204000000</v>
+      </c>
+      <c r="AU19">
+        <v>12204000000</v>
+      </c>
+      <c r="AV19">
+        <v>17315000000</v>
+      </c>
+      <c r="AW19">
+        <v>0</v>
+      </c>
+      <c r="AX19">
+        <v>17315000000</v>
+      </c>
+      <c r="AY19">
+        <v>0</v>
+      </c>
+      <c r="AZ19">
+        <v>2643000000</v>
+      </c>
+      <c r="BA19">
+        <v>-8253000000</v>
+      </c>
+      <c r="BB19" s="3" t="s">
+        <v>153</v>
+      </c>
+      <c r="BC19" s="3" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="20" spans="1:55">
+      <c r="A20" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="B20" s="2">
+        <v>44227</v>
+      </c>
+      <c r="C20" t="s">
+        <v>75</v>
+      </c>
+      <c r="D20" t="s">
+        <v>76</v>
+      </c>
+      <c r="E20" t="s">
+        <v>77</v>
+      </c>
+      <c r="F20" t="s">
+        <v>96</v>
+      </c>
+      <c r="G20" t="s">
+        <v>116</v>
+      </c>
+      <c r="H20" t="s">
+        <v>136</v>
+      </c>
+      <c r="I20" t="s">
+        <v>138</v>
+      </c>
+      <c r="J20">
+        <v>847000000</v>
+      </c>
+      <c r="K20">
+        <v>10714000000</v>
+      </c>
+      <c r="L20">
+        <v>11561000000</v>
+      </c>
+      <c r="M20">
+        <v>2429000000</v>
+      </c>
+      <c r="N20">
+        <v>1826000000</v>
+      </c>
+      <c r="O20">
+        <v>239000000</v>
+      </c>
+      <c r="P20">
+        <v>16055000000</v>
+      </c>
+      <c r="Q20">
+        <v>2856000000</v>
+      </c>
+      <c r="R20">
+        <v>4193000000</v>
+      </c>
+      <c r="S20">
+        <v>2737000000</v>
+      </c>
+      <c r="T20">
+        <v>6930000000</v>
+      </c>
+      <c r="U20">
+        <v>144000000</v>
+      </c>
+      <c r="V20">
+        <v>806000000</v>
+      </c>
+      <c r="W20">
+        <v>2000000000</v>
+      </c>
+      <c r="X20">
+        <v>12736000000</v>
+      </c>
+      <c r="Y20">
+        <v>0</v>
+      </c>
+      <c r="Z20">
+        <v>28791000000</v>
+      </c>
+      <c r="AA20">
+        <v>1201000000</v>
+      </c>
+      <c r="AB20">
+        <v>1120000000</v>
+      </c>
+      <c r="AC20">
+        <v>61000000</v>
+      </c>
+      <c r="AD20">
+        <v>288000000</v>
+      </c>
+      <c r="AE20">
+        <v>1255000000</v>
+      </c>
+      <c r="AF20">
+        <v>3925000000</v>
+      </c>
+      <c r="AG20">
+        <v>6598000000</v>
+      </c>
+      <c r="AH20">
+        <v>163000000</v>
+      </c>
+      <c r="AI20">
+        <v>241000000</v>
+      </c>
+      <c r="AJ20">
+        <v>971000000</v>
+      </c>
+      <c r="AK20">
+        <v>7973000000</v>
+      </c>
+      <c r="AL20">
+        <v>0</v>
+      </c>
+      <c r="AM20">
+        <v>755000000</v>
+      </c>
+      <c r="AN20">
+        <v>11898000000</v>
+      </c>
+      <c r="AO20">
+        <v>0</v>
+      </c>
+      <c r="AP20">
+        <v>1000000</v>
+      </c>
+      <c r="AQ20">
+        <v>18908000000</v>
+      </c>
+      <c r="AR20">
+        <v>19000000</v>
+      </c>
+      <c r="AS20">
+        <v>-2035000000</v>
+      </c>
+      <c r="AT20">
+        <v>16893000000</v>
+      </c>
+      <c r="AU20">
+        <v>16893000000</v>
+      </c>
+      <c r="AV20">
+        <v>28791000000</v>
+      </c>
+      <c r="AW20">
+        <v>0</v>
+      </c>
+      <c r="AX20">
+        <v>28791000000</v>
+      </c>
+      <c r="AY20">
+        <v>10858000000</v>
+      </c>
+      <c r="AZ20">
+        <v>7718000000</v>
+      </c>
+      <c r="BA20">
+        <v>6871000000</v>
+      </c>
+      <c r="BB20" s="3" t="s">
+        <v>154</v>
+      </c>
+      <c r="BC20" s="3" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="21" spans="1:55">
+      <c r="A21" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="B21" s="2">
         <v>44591</v>
       </c>
-      <c r="C11" t="s">
-        <v>65</v>
-      </c>
-      <c r="D11" t="s">
-        <v>66</v>
-      </c>
-      <c r="E11" t="s">
-        <v>67</v>
-      </c>
-      <c r="F11" t="s">
+      <c r="C21" t="s">
+        <v>75</v>
+      </c>
+      <c r="D21" t="s">
+        <v>76</v>
+      </c>
+      <c r="E21" t="s">
         <v>77</v>
       </c>
-      <c r="G11" t="s">
-        <v>87</v>
-      </c>
-      <c r="H11" t="s">
+      <c r="F21" t="s">
         <v>97</v>
       </c>
-      <c r="I11" t="s">
-        <v>98</v>
-      </c>
-      <c r="J11">
+      <c r="G21" t="s">
+        <v>117</v>
+      </c>
+      <c r="H21" t="s">
+        <v>137</v>
+      </c>
+      <c r="I21" t="s">
+        <v>138</v>
+      </c>
+      <c r="J21">
         <v>1990000000</v>
       </c>
-      <c r="K11">
+      <c r="K21">
         <v>19218000000</v>
       </c>
-      <c r="L11">
+      <c r="L21">
         <v>21208000000</v>
       </c>
-      <c r="M11">
+      <c r="M21">
         <v>4650000000</v>
       </c>
-      <c r="N11">
+      <c r="N21">
         <v>2605000000</v>
       </c>
-      <c r="O11">
+      <c r="O21">
         <v>366000000</v>
       </c>
-      <c r="P11">
+      <c r="P21">
         <v>28829000000</v>
       </c>
-      <c r="Q11">
+      <c r="Q21">
         <v>3607000000</v>
       </c>
-      <c r="R11">
+      <c r="R21">
         <v>4349000000</v>
       </c>
-      <c r="S11">
+      <c r="S21">
         <v>2339000000</v>
       </c>
-      <c r="T11">
+      <c r="T21">
         <v>6688000000</v>
       </c>
-      <c r="U11">
+      <c r="U21">
         <v>266000000</v>
       </c>
-      <c r="V11">
+      <c r="V21">
         <v>1222000000</v>
       </c>
-      <c r="W11">
+      <c r="W21">
         <v>3575000000</v>
       </c>
-      <c r="X11">
+      <c r="X21">
         <v>15358000000</v>
       </c>
-      <c r="Y11">
-        <v>0</v>
-      </c>
-      <c r="Z11">
+      <c r="Y21">
+        <v>0</v>
+      </c>
+      <c r="Z21">
         <v>44187000000</v>
       </c>
-      <c r="AA11">
+      <c r="AA21">
         <v>1783000000</v>
       </c>
-      <c r="AB11">
-        <v>0</v>
-      </c>
-      <c r="AC11">
-        <v>0</v>
-      </c>
-      <c r="AD11">
+      <c r="AB21">
+        <v>0</v>
+      </c>
+      <c r="AC21">
+        <v>0</v>
+      </c>
+      <c r="AD21">
         <v>300000000</v>
       </c>
-      <c r="AE11">
+      <c r="AE21">
         <v>2252000000</v>
       </c>
-      <c r="AF11">
+      <c r="AF21">
         <v>4335000000</v>
       </c>
-      <c r="AG11">
+      <c r="AG21">
         <v>11687000000</v>
       </c>
-      <c r="AH11">
+      <c r="AH21">
         <v>202000000</v>
       </c>
-      <c r="AI11">
+      <c r="AI21">
         <v>245000000</v>
       </c>
-      <c r="AJ11">
+      <c r="AJ21">
         <v>1106000000</v>
       </c>
-      <c r="AK11">
+      <c r="AK21">
         <v>13240000000</v>
       </c>
-      <c r="AL11">
-        <v>0</v>
-      </c>
-      <c r="AM11">
+      <c r="AL21">
+        <v>0</v>
+      </c>
+      <c r="AM21">
         <v>741000000</v>
       </c>
-      <c r="AN11">
+      <c r="AN21">
         <v>17575000000</v>
       </c>
-      <c r="AO11">
-        <v>0</v>
-      </c>
-      <c r="AP11">
+      <c r="AO21">
+        <v>0</v>
+      </c>
+      <c r="AP21">
         <v>3000000</v>
       </c>
-      <c r="AQ11">
+      <c r="AQ21">
         <v>16235000000</v>
       </c>
-      <c r="AR11">
+      <c r="AR21">
         <v>-11000000</v>
       </c>
-      <c r="AS11">
+      <c r="AS21">
         <v>10385000000</v>
       </c>
-      <c r="AT11">
+      <c r="AT21">
         <v>26612000000</v>
       </c>
-      <c r="AU11">
+      <c r="AU21">
         <v>26612000000</v>
       </c>
-      <c r="AV11">
+      <c r="AV21">
         <v>44187000000</v>
       </c>
-      <c r="AW11">
-        <v>0</v>
-      </c>
-      <c r="AX11">
+      <c r="AW21">
+        <v>0</v>
+      </c>
+      <c r="AX21">
         <v>44187000000</v>
       </c>
-      <c r="AY11">
+      <c r="AY21">
         <v>19484000000</v>
       </c>
-      <c r="AZ11">
+      <c r="AZ21">
         <v>11687000000</v>
       </c>
-      <c r="BA11">
+      <c r="BA21">
         <v>9697000000</v>
       </c>
-      <c r="BB11" s="3" t="s">
-        <v>108</v>
-      </c>
-      <c r="BC11" s="3" t="s">
-        <v>116</v>
+      <c r="BB21" s="3" t="s">
+        <v>155</v>
+      </c>
+      <c r="BC21" s="3" t="s">
+        <v>167</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="BB2" r:id="rId1"/>
     <hyperlink ref="BC2" r:id="rId2"/>
-    <hyperlink ref="BB3" r:id="rId3"/>
-    <hyperlink ref="BC3" r:id="rId4"/>
-    <hyperlink ref="BB4" r:id="rId5"/>
-    <hyperlink ref="BC4" r:id="rId6"/>
-    <hyperlink ref="BB5" r:id="rId7"/>
-    <hyperlink ref="BC5" r:id="rId8"/>
-    <hyperlink ref="BB6" r:id="rId9"/>
-    <hyperlink ref="BC6" r:id="rId10"/>
-    <hyperlink ref="BB7" r:id="rId11"/>
-    <hyperlink ref="BC7" r:id="rId12"/>
-    <hyperlink ref="BB8" r:id="rId13"/>
-    <hyperlink ref="BC8" r:id="rId14"/>
-    <hyperlink ref="BB9" r:id="rId15"/>
-    <hyperlink ref="BC9" r:id="rId16"/>
-    <hyperlink ref="BB10" r:id="rId17"/>
-    <hyperlink ref="BC10" r:id="rId18"/>
-    <hyperlink ref="BB11" r:id="rId19"/>
-    <hyperlink ref="BC11" r:id="rId20"/>
+    <hyperlink ref="BB4" r:id="rId3"/>
+    <hyperlink ref="BC4" r:id="rId4"/>
+    <hyperlink ref="BB5" r:id="rId5"/>
+    <hyperlink ref="BC5" r:id="rId6"/>
+    <hyperlink ref="BB6" r:id="rId7"/>
+    <hyperlink ref="BC6" r:id="rId8"/>
+    <hyperlink ref="BB9" r:id="rId9"/>
+    <hyperlink ref="BC9" r:id="rId10"/>
+    <hyperlink ref="BB10" r:id="rId11"/>
+    <hyperlink ref="BC10" r:id="rId12"/>
+    <hyperlink ref="BB11" r:id="rId13"/>
+    <hyperlink ref="BC11" r:id="rId14"/>
+    <hyperlink ref="BB12" r:id="rId15"/>
+    <hyperlink ref="BC12" r:id="rId16"/>
+    <hyperlink ref="BB13" r:id="rId17"/>
+    <hyperlink ref="BC13" r:id="rId18"/>
+    <hyperlink ref="BB14" r:id="rId19"/>
+    <hyperlink ref="BC14" r:id="rId20"/>
+    <hyperlink ref="BB15" r:id="rId21"/>
+    <hyperlink ref="BC15" r:id="rId22"/>
+    <hyperlink ref="BB16" r:id="rId23"/>
+    <hyperlink ref="BC16" r:id="rId24"/>
+    <hyperlink ref="BB17" r:id="rId25"/>
+    <hyperlink ref="BC17" r:id="rId26"/>
+    <hyperlink ref="BB18" r:id="rId27"/>
+    <hyperlink ref="BC18" r:id="rId28"/>
+    <hyperlink ref="BB19" r:id="rId29"/>
+    <hyperlink ref="BC19" r:id="rId30"/>
+    <hyperlink ref="BB20" r:id="rId31"/>
+    <hyperlink ref="BC20" r:id="rId32"/>
+    <hyperlink ref="BB21" r:id="rId33"/>
+    <hyperlink ref="BC21" r:id="rId34"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>